<commit_message>
Add CRS To RTM
</commit_message>
<xml_diff>
--- a/management/RTM.xlsx
+++ b/management/RTM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammad Elzeiny\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Embedded Systems\iTi Program\Software Engineer\Project\Kenovo_ElectricBlender\management\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9336" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
   <si>
     <t>REQUIREMENTS TRACEABILITY MATRIX</t>
   </si>
@@ -242,69 +242,6 @@
   </si>
   <si>
     <t>013</t>
-  </si>
-  <si>
-    <t>014</t>
-  </si>
-  <si>
-    <t>015</t>
-  </si>
-  <si>
-    <t>016</t>
-  </si>
-  <si>
-    <t>017</t>
-  </si>
-  <si>
-    <t>018</t>
-  </si>
-  <si>
-    <t>019</t>
-  </si>
-  <si>
-    <t>020</t>
-  </si>
-  <si>
-    <t>021</t>
-  </si>
-  <si>
-    <t>022</t>
-  </si>
-  <si>
-    <t>023</t>
-  </si>
-  <si>
-    <t>024</t>
-  </si>
-  <si>
-    <t>025</t>
-  </si>
-  <si>
-    <t>026</t>
-  </si>
-  <si>
-    <t>027</t>
-  </si>
-  <si>
-    <t>028</t>
-  </si>
-  <si>
-    <t>029</t>
-  </si>
-  <si>
-    <t>030</t>
-  </si>
-  <si>
-    <t>031</t>
-  </si>
-  <si>
-    <t>032</t>
-  </si>
-  <si>
-    <t>033</t>
-  </si>
-  <si>
-    <t>034</t>
   </si>
   <si>
     <t>Function (in code)</t>
@@ -459,12 +396,90 @@
       <t>: This column should be populated with any additional comments</t>
     </r>
   </si>
+  <si>
+    <t>REQ_1</t>
+  </si>
+  <si>
+    <t>REQ_2</t>
+  </si>
+  <si>
+    <t>REQ_3</t>
+  </si>
+  <si>
+    <t>REQ_4</t>
+  </si>
+  <si>
+    <t>REQ_5</t>
+  </si>
+  <si>
+    <t>REQ_6</t>
+  </si>
+  <si>
+    <t>REQ_7</t>
+  </si>
+  <si>
+    <t>REQ_8</t>
+  </si>
+  <si>
+    <t>REQ_9</t>
+  </si>
+  <si>
+    <t>REQ_10</t>
+  </si>
+  <si>
+    <t>REQ_11</t>
+  </si>
+  <si>
+    <t>REQ_12</t>
+  </si>
+  <si>
+    <t>REQ_13</t>
+  </si>
+  <si>
+    <t>The initial state of the blender is OFF</t>
+  </si>
+  <si>
+    <t>The blender rotate in one direction</t>
+  </si>
+  <si>
+    <t>There is no power button for blender</t>
+  </si>
+  <si>
+    <t>Additional hardware can be used to detect the over-voltage state</t>
+  </si>
+  <si>
+    <t>If the voltage exceeds motor operating voltage it will stop</t>
+  </si>
+  <si>
+    <t>Motor operating voltage is between 5 to 9V.</t>
+  </si>
+  <si>
+    <t>Motor should remain off in case of over-voltage condition.</t>
+  </si>
+  <si>
+    <t>the speeds percentage are the same</t>
+  </si>
+  <si>
+    <t>Speed remains the same if user pressed button forever</t>
+  </si>
+  <si>
+    <t>Blender stays active with current speed unless user changes its operating state using button.</t>
+  </si>
+  <si>
+    <t>Button used is tactile switch</t>
+  </si>
+  <si>
+    <t>Action is immediately taken after button release with no delays.</t>
+  </si>
+  <si>
+    <t>Must press button and release it to initiate action.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,8 +555,29 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -569,6 +605,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -649,10 +691,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -674,6 +717,24 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -699,18 +760,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -1013,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1023,58 +1075,58 @@
     <col min="2" max="2" width="8.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:1" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" s="17" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" s="17" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" s="18" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" s="17" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" s="17" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="17" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" s="17" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="17" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:1" s="13" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="13" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="15" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="13" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="13" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A8:XFD8"/>
@@ -1097,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1114,31 +1166,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.25">
@@ -1155,7 +1207,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>7</v>
@@ -1172,7 +1224,9 @@
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -1185,7 +1239,9 @@
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -1198,7 +1254,9 @@
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -1211,7 +1269,9 @@
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1224,7 +1284,9 @@
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1237,7 +1299,9 @@
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1250,7 +1314,9 @@
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1263,7 +1329,9 @@
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1276,7 +1344,9 @@
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1289,7 +1359,9 @@
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1302,7 +1374,9 @@
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1315,7 +1389,9 @@
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="12" t="s">
+        <v>45</v>
+      </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1328,7 +1404,9 @@
       <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="12" t="s">
+        <v>46</v>
+      </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1338,10 +1416,8 @@
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="6"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1351,9 +1427,7 @@
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1364,9 +1438,7 @@
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1377,9 +1449,7 @@
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1390,9 +1460,7 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1403,9 +1471,7 @@
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1416,9 +1482,7 @@
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1429,9 +1493,7 @@
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1442,9 +1504,7 @@
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1455,9 +1515,7 @@
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1468,9 +1526,7 @@
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1481,9 +1537,7 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1494,9 +1548,7 @@
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1507,9 +1559,7 @@
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1520,9 +1570,7 @@
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1533,9 +1581,7 @@
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1546,9 +1592,7 @@
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1559,9 +1603,7 @@
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1572,9 +1614,7 @@
       <c r="I34" s="2"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1585,9 +1625,7 @@
       <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1598,9 +1636,7 @@
       <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1946,19 +1982,146 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B4" location="CRS!A2" display="Req_1"/>
+    <hyperlink ref="B5" location="CRS!A3" display="REQ_2"/>
+    <hyperlink ref="B6" location="CRS!A4" display="REQ_3"/>
+    <hyperlink ref="B7" location="CRS!A5" display="REQ_4"/>
+    <hyperlink ref="B8" location="CRS!A6" display="REQ_5"/>
+    <hyperlink ref="B9" location="CRS!A7" display="REQ_6"/>
+    <hyperlink ref="B10" location="CRS!A8" display="REQ_7"/>
+    <hyperlink ref="B11" location="CRS!A9" display="REQ_8"/>
+    <hyperlink ref="B12" location="CRS!A10" display="REQ_9"/>
+    <hyperlink ref="B13" location="CRS!A11" display="REQ_10"/>
+    <hyperlink ref="B14" location="CRS!A12" display="REQ_11"/>
+    <hyperlink ref="B15" location="CRS!A13" display="REQ_12"/>
+    <hyperlink ref="B16" location="CRS!A14" display="REQ_13"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="74.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updating RTM with new CRS ids and SRS ids
</commit_message>
<xml_diff>
--- a/management/RTM.xlsx
+++ b/management/RTM.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Embedded Systems\iTi Program\Software Engineer\Project\Kenovo_ElectricBlender\management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA_Embedded_project\Kenovo_ElectricBlender\management\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
   <si>
     <t>REQUIREMENTS TRACEABILITY MATRIX</t>
   </si>
@@ -257,7 +257,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -272,7 +272,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -287,7 +287,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -322,7 +322,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -337,7 +337,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -352,7 +352,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -389,7 +389,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -406,36 +406,6 @@
     <t>REQ_3</t>
   </si>
   <si>
-    <t>REQ_4</t>
-  </si>
-  <si>
-    <t>REQ_5</t>
-  </si>
-  <si>
-    <t>REQ_6</t>
-  </si>
-  <si>
-    <t>REQ_7</t>
-  </si>
-  <si>
-    <t>REQ_8</t>
-  </si>
-  <si>
-    <t>REQ_9</t>
-  </si>
-  <si>
-    <t>REQ_10</t>
-  </si>
-  <si>
-    <t>REQ_11</t>
-  </si>
-  <si>
-    <t>REQ_12</t>
-  </si>
-  <si>
-    <t>REQ_13</t>
-  </si>
-  <si>
     <t>The initial state of the blender is OFF</t>
   </si>
   <si>
@@ -473,17 +443,74 @@
   </si>
   <si>
     <t>Must press button and release it to initiate action.</t>
+  </si>
+  <si>
+    <t>SRS_1 - SRS_2 - SRS_6 - SRS_8 - SRS_9 - SRS_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRS_4 - SRS_5 - SRS_6 - SRS_7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRS_3 - SRS_9 - SRS_10 - SRS_11 - SRS_12 - SRS_13 </t>
+  </si>
+  <si>
+    <t>A blender with three different speeds.</t>
+  </si>
+  <si>
+    <t>Blender is protected from over-voltage.</t>
+  </si>
+  <si>
+    <t>Blender is controlled using one button.</t>
+  </si>
+  <si>
+    <t>SRS_1</t>
+  </si>
+  <si>
+    <t>SRS_2</t>
+  </si>
+  <si>
+    <t>SRS_3</t>
+  </si>
+  <si>
+    <t>SRS_4</t>
+  </si>
+  <si>
+    <t>SRS_5</t>
+  </si>
+  <si>
+    <t>SRS_6</t>
+  </si>
+  <si>
+    <t>SRS_7</t>
+  </si>
+  <si>
+    <t>SRS_8</t>
+  </si>
+  <si>
+    <t>SRS_9</t>
+  </si>
+  <si>
+    <t>SRS_10</t>
+  </si>
+  <si>
+    <t>SRS_11</t>
+  </si>
+  <si>
+    <t>SRS_12</t>
+  </si>
+  <si>
+    <t>SRS_13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -526,7 +553,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -558,7 +585,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -572,9 +599,15 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -695,7 +728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -722,9 +755,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -758,6 +788,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1069,64 +1106,64 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.796875" customWidth="1"/>
-    <col min="2" max="2" width="8.796875" customWidth="1"/>
+    <col min="1" max="1" width="30.77734375" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:1" s="13" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="2" spans="1:1" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:1" s="12" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="13" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:1" s="12" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:1" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="15" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:1" s="14" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:1" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="13" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:1" s="12" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:1" s="12" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:1" s="12" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="13" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:1" s="12" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A8:XFD8"/>
@@ -1149,51 +1186,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.19921875" customWidth="1"/>
-    <col min="2" max="2" width="32.59765625" customWidth="1"/>
-    <col min="3" max="3" width="35.3984375" customWidth="1"/>
-    <col min="4" max="4" width="26.296875" customWidth="1"/>
+    <col min="1" max="1" width="7.21875" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="18.59765625" customWidth="1"/>
-    <col min="7" max="7" width="20.296875" customWidth="1"/>
-    <col min="8" max="8" width="18.796875" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="23"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1220,14 +1257,16 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -1235,14 +1274,16 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -1250,14 +1291,16 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -1265,13 +1308,11 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="B7" s="11"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1280,13 +1321,11 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="B8" s="11"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1295,13 +1334,11 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="B9" s="11"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1310,13 +1347,11 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="B10" s="11"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1325,13 +1360,11 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="B11" s="11"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1340,13 +1373,11 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>42</v>
-      </c>
+      <c r="B12" s="11"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1355,13 +1386,11 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>43</v>
-      </c>
+      <c r="B13" s="11"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1370,13 +1399,11 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>44</v>
-      </c>
+      <c r="B14" s="11"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1385,13 +1412,11 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="B15" s="11"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1400,13 +1425,11 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>46</v>
-      </c>
+      <c r="B16" s="11"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1415,7 +1438,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="10"/>
       <c r="C17" s="7"/>
@@ -1426,7 +1449,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -1437,7 +1460,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
@@ -1448,7 +1471,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -1459,7 +1482,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -1470,7 +1493,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
@@ -1481,7 +1504,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
@@ -1492,7 +1515,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
@@ -1503,7 +1526,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
@@ -1514,7 +1537,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
@@ -1525,7 +1548,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
@@ -1536,7 +1559,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
@@ -1547,7 +1570,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
@@ -1558,7 +1581,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
@@ -1569,7 +1592,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
@@ -1580,7 +1603,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
@@ -1591,7 +1614,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
@@ -1602,7 +1625,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
@@ -1613,7 +1636,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
@@ -1624,7 +1647,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
@@ -1635,7 +1658,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
@@ -1646,7 +1669,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1657,7 +1680,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1668,7 +1691,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1679,7 +1702,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1690,7 +1713,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1701,7 +1724,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1712,7 +1735,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1723,7 +1746,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1734,7 +1757,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1745,7 +1768,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1756,7 +1779,7 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1767,7 +1790,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -1778,7 +1801,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -1789,7 +1812,7 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -1800,7 +1823,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -1811,7 +1834,7 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -1822,7 +1845,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -1833,7 +1856,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -1844,7 +1867,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -1855,7 +1878,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -1866,7 +1889,7 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -1877,7 +1900,7 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -1888,7 +1911,7 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -1899,7 +1922,7 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -1910,7 +1933,7 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -1921,7 +1944,7 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -1932,7 +1955,7 @@
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -1943,7 +1966,7 @@
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -1954,7 +1977,7 @@
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -1986,16 +2009,6 @@
     <hyperlink ref="B4" location="CRS!A2" display="Req_1"/>
     <hyperlink ref="B5" location="CRS!A3" display="REQ_2"/>
     <hyperlink ref="B6" location="CRS!A4" display="REQ_3"/>
-    <hyperlink ref="B7" location="CRS!A5" display="REQ_4"/>
-    <hyperlink ref="B8" location="CRS!A6" display="REQ_5"/>
-    <hyperlink ref="B9" location="CRS!A7" display="REQ_6"/>
-    <hyperlink ref="B10" location="CRS!A8" display="REQ_7"/>
-    <hyperlink ref="B11" location="CRS!A9" display="REQ_8"/>
-    <hyperlink ref="B12" location="CRS!A10" display="REQ_9"/>
-    <hyperlink ref="B13" location="CRS!A11" display="REQ_10"/>
-    <hyperlink ref="B14" location="CRS!A12" display="REQ_11"/>
-    <hyperlink ref="B15" location="CRS!A13" display="REQ_12"/>
-    <hyperlink ref="B16" location="CRS!A14" display="REQ_13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2005,120 +2018,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="74.3984375" customWidth="1"/>
+    <col min="2" max="2" width="74.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B4" s="25" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2128,12 +2061,119 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2144,7 +2184,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating RTM with test cases and their ids
</commit_message>
<xml_diff>
--- a/management/RTM.xlsx
+++ b/management/RTM.xlsx
@@ -18,7 +18,7 @@
     <sheet name="SRS" sheetId="4" r:id="rId4"/>
     <sheet name="Test Cases" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,6 +64,7 @@
             <sz val="8"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">• Assoc ID: </t>
         </r>
@@ -86,6 +87,7 @@
             <sz val="8"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">• Technical Assumptions or Customer Needs:  </t>
         </r>
@@ -108,6 +110,7 @@
             <sz val="8"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">• Architectural/Design Document:  </t>
         </r>
@@ -153,6 +156,7 @@
             <sz val="8"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">• System Component(s):  </t>
         </r>
@@ -172,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
   <si>
     <t>REQUIREMENTS TRACEABILITY MATRIX</t>
   </si>
@@ -445,15 +449,6 @@
     <t>Must press button and release it to initiate action.</t>
   </si>
   <si>
-    <t>SRS_1 - SRS_2 - SRS_6 - SRS_8 - SRS_9 - SRS_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRS_4 - SRS_5 - SRS_6 - SRS_7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRS_3 - SRS_9 - SRS_10 - SRS_11 - SRS_12 - SRS_13 </t>
-  </si>
-  <si>
     <t>A blender with three different speeds.</t>
   </si>
   <si>
@@ -500,13 +495,122 @@
   </si>
   <si>
     <t>SRS_13</t>
+  </si>
+  <si>
+    <t>TC_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> validate button pressing</t>
+  </si>
+  <si>
+    <t>TC_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> validate Speed 1</t>
+  </si>
+  <si>
+    <t>TC_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> validate Speed 2</t>
+  </si>
+  <si>
+    <t>TC_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> validate Speed 3</t>
+  </si>
+  <si>
+    <t>TC_5</t>
+  </si>
+  <si>
+    <t>Validate Pressing on button frequently.</t>
+  </si>
+  <si>
+    <t>TC_6</t>
+  </si>
+  <si>
+    <t>Validate Long Press on the button.</t>
+  </si>
+  <si>
+    <t>TC_7</t>
+  </si>
+  <si>
+    <t>validate motor rotation</t>
+  </si>
+  <si>
+    <t>TC_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Protection circuit </t>
+  </si>
+  <si>
+    <t>TC _9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify the PWM Voltage </t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>Verify the initial state of the blender.</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>Verify No Power Button.</t>
+  </si>
+  <si>
+    <t>- SRS_1 - 
+- SRS_2 - 
+- SRS_6 - 
+- SRS_8 - 
+- SRS_9 - 
+- SRS_10</t>
+  </si>
+  <si>
+    <t>- SRS_4 - 
+- SRS_5 - 
+- SRS_6 -
+- SRS_7 -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- SRS_3 - 
+- SRS_9 - 
+- SRS_10 - 
+- SRS_11 - 
+- SRS_12 - 
+- SRS_13 - </t>
+  </si>
+  <si>
+    <t>- TC_10 - 
+- TC_7 - 
+- TC_8 -  
+- TC_9 -  
+- TC_6 - 
+- TC_1 -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- TC_8 - 
+- TC_8 - 
+- TC_8 - 
+- TC_8 - </t>
+  </si>
+  <si>
+    <t>- TC_11 - 
+- TC_6 - 
+- TC_1 - 
+- TC_1 - 
+- TC_5 -</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,12 +649,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -583,19 +681,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -608,6 +693,38 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -724,11 +841,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -753,19 +871,41 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -790,17 +930,18 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1112,54 +1253,54 @@
     <col min="2" max="2" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:1" s="12" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="2" spans="1:1" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:1" s="20" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="12" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:1" s="20" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:1" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="14" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:1" s="22" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:1" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="12" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:1" s="20" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="12" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:1" s="20" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="12" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:1" s="20" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="12" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:1" s="20" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1186,48 +1327,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.21875" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
-    <col min="3" max="3" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" style="19" customWidth="1"/>
     <col min="4" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
     <col min="7" max="7" width="20.33203125" customWidth="1"/>
     <col min="8" max="8" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1257,53 +1398,59 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>92</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="129" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>93</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1312,7 +1459,7 @@
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1325,7 +1472,7 @@
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1338,7 +1485,7 @@
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1351,7 +1498,7 @@
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1364,7 +1511,7 @@
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1377,7 +1524,7 @@
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1390,7 +1537,7 @@
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="11"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1403,7 +1550,7 @@
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="11"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1416,7 +1563,7 @@
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1429,7 +1576,7 @@
       <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1440,7 +1587,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
-      <c r="B17" s="10"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1451,7 +1598,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1462,7 +1609,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1473,7 +1620,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -1484,7 +1631,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -1495,7 +1642,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -1506,7 +1653,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1517,7 +1664,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -1528,7 +1675,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -1539,7 +1686,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -1550,7 +1697,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
+      <c r="B27" s="17"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -1561,7 +1708,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -1572,7 +1719,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
@@ -1583,7 +1730,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
@@ -1594,7 +1741,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -1605,7 +1752,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -1616,7 +1763,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -1627,7 +1774,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -1638,7 +1785,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
+      <c r="B35" s="17"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -1649,7 +1796,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
+      <c r="B36" s="17"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -1660,7 +1807,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -1671,7 +1818,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
+      <c r="B38" s="17"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -1682,7 +1829,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
+      <c r="B39" s="17"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -1693,7 +1840,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
+      <c r="B40" s="17"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -1704,7 +1851,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
+      <c r="B41" s="17"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -1715,7 +1862,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
+      <c r="B42" s="17"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -1726,7 +1873,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
+      <c r="B43" s="17"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -1737,7 +1884,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
+      <c r="B44" s="17"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -1748,7 +1895,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
+      <c r="B45" s="17"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -1759,7 +1906,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
+      <c r="B46" s="17"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -1770,7 +1917,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
+      <c r="B47" s="17"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
@@ -1781,7 +1928,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -1792,7 +1939,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -1803,7 +1950,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
+      <c r="B50" s="17"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
@@ -1814,7 +1961,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
+      <c r="B51" s="17"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -1825,7 +1972,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
+      <c r="B52" s="17"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -1836,7 +1983,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
+      <c r="B53" s="17"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -1847,7 +1994,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
+      <c r="B54" s="17"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -1858,7 +2005,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
+      <c r="B55" s="17"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
@@ -1869,7 +2016,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
+      <c r="B56" s="17"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -1880,7 +2027,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
-      <c r="B57" s="6"/>
+      <c r="B57" s="17"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
@@ -1891,7 +2038,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
+      <c r="B58" s="17"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
@@ -1902,7 +2049,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
-      <c r="B59" s="6"/>
+      <c r="B59" s="17"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
@@ -1913,7 +2060,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
-      <c r="B60" s="6"/>
+      <c r="B60" s="17"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
@@ -1924,7 +2071,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
-      <c r="B61" s="6"/>
+      <c r="B61" s="17"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
@@ -1935,7 +2082,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
+      <c r="B62" s="17"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
@@ -1946,7 +2093,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
-      <c r="B63" s="6"/>
+      <c r="B63" s="17"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
@@ -1957,7 +2104,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
-      <c r="B64" s="6"/>
+      <c r="B64" s="17"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
@@ -1968,7 +2115,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
-      <c r="B65" s="6"/>
+      <c r="B65" s="17"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
@@ -1979,7 +2126,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
-      <c r="B66" s="6"/>
+      <c r="B66" s="17"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
@@ -2034,24 +2181,24 @@
       <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>53</v>
+      <c r="B2" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>54</v>
+      <c r="B3" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>55</v>
+      <c r="B4" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2064,14 +2211,14 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
         <v>37</v>
@@ -2079,7 +2226,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -2087,7 +2234,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -2095,7 +2242,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
@@ -2103,7 +2250,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
@@ -2111,7 +2258,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
@@ -2119,7 +2266,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
@@ -2127,7 +2274,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
@@ -2135,7 +2282,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>45</v>
@@ -2143,7 +2290,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
         <v>46</v>
@@ -2151,7 +2298,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
         <v>47</v>
@@ -2159,7 +2306,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
         <v>48</v>
@@ -2167,7 +2314,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
         <v>49</v>
@@ -2180,12 +2327,189 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+    </row>
+    <row r="25" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="13"/>
+    </row>
+    <row r="27" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="13"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="B10:B14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated RTM with the new SRS and their relevant ids only and didnt change any testcase or any ids for them
</commit_message>
<xml_diff>
--- a/management/RTM.xlsx
+++ b/management/RTM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9336" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9336" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
   <si>
     <t>REQUIREMENTS TRACEABILITY MATRIX</t>
   </si>
@@ -419,36 +419,9 @@
     <t>There is no power button for blender</t>
   </si>
   <si>
-    <t>Additional hardware can be used to detect the over-voltage state</t>
-  </si>
-  <si>
-    <t>If the voltage exceeds motor operating voltage it will stop</t>
-  </si>
-  <si>
-    <t>Motor operating voltage is between 5 to 9V.</t>
-  </si>
-  <si>
-    <t>Motor should remain off in case of over-voltage condition.</t>
-  </si>
-  <si>
-    <t>the speeds percentage are the same</t>
-  </si>
-  <si>
-    <t>Speed remains the same if user pressed button forever</t>
-  </si>
-  <si>
-    <t>Blender stays active with current speed unless user changes its operating state using button.</t>
-  </si>
-  <si>
     <t>Button used is tactile switch</t>
   </si>
   <si>
-    <t>Action is immediately taken after button release with no delays.</t>
-  </si>
-  <si>
-    <t>Must press button and release it to initiate action.</t>
-  </si>
-  <si>
     <t>A blender with three different speeds.</t>
   </si>
   <si>
@@ -494,9 +467,6 @@
     <t>SRS_12</t>
   </si>
   <si>
-    <t>SRS_13</t>
-  </si>
-  <si>
     <t>TC_1</t>
   </si>
   <si>
@@ -561,28 +531,6 @@
   </si>
   <si>
     <t>Verify No Power Button.</t>
-  </si>
-  <si>
-    <t>- SRS_1 - 
-- SRS_2 - 
-- SRS_6 - 
-- SRS_8 - 
-- SRS_9 - 
-- SRS_10</t>
-  </si>
-  <si>
-    <t>- SRS_4 - 
-- SRS_5 - 
-- SRS_6 -
-- SRS_7 -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- SRS_3 - 
-- SRS_9 - 
-- SRS_10 - 
-- SRS_11 - 
-- SRS_12 - 
-- SRS_13 - </t>
   </si>
   <si>
     <t>- TC_10 - 
@@ -605,12 +553,57 @@
 - TC_1 - 
 - TC_5 -</t>
   </si>
+  <si>
+    <t>Motor operating voltage is between 5 to 9V</t>
+  </si>
+  <si>
+    <t>Additional hardware is used to detect the over-voltage state. If voltage exceeds motor operating voltage [5 to 9 V], the motor stops and system shuts down</t>
+  </si>
+  <si>
+    <t>Speed remains the same if user pressed button for more than one second</t>
+  </si>
+  <si>
+    <t>Action is taken after button pressed and released in interval bigger than 1/3 second and less than one second.</t>
+  </si>
+  <si>
+    <t>Frequent button press is described as button pressing and releasing in interval less than 1/3 second</t>
+  </si>
+  <si>
+    <t>Blender stays active with current speed unless user changes its operating state using button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action is taken after button release with no delays observed by the human </t>
+  </si>
+  <si>
+    <t>- SRS_6 -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- SRS_1 - 
+- SRS_2 - 
+- SRS_3 -
+- SRS_7 -
+- SRS_8 -
+- SRS_9 -
+- SRS_10 -
+- SRS_11 -
+- SRS_12 -
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- SRS_4 - 
+- SRS_5 - 
+</t>
+  </si>
+  <si>
+    <t>speeds variation must be observed clearly by vision and sound</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -725,6 +718,13 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -846,7 +846,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -937,6 +937,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1327,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1398,39 +1402,39 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="34" t="s">
         <v>88</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="34" t="s">
         <v>89</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -1443,13 +1447,13 @@
       <c r="B6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="34" t="s">
         <v>90</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2182,7 +2186,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -2190,7 +2194,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -2198,7 +2202,7 @@
         <v>36</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2208,120 +2212,116 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B10" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B11" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" t="s">
-        <v>49</v>
+      <c r="B12" s="19" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2341,42 +2341,42 @@
   <sheetData>
     <row r="1" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2397,10 +2397,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2421,10 +2421,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -2449,10 +2449,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -2467,12 +2467,12 @@
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
     </row>
-    <row r="25" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -2481,10 +2481,10 @@
     </row>
     <row r="27" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2493,10 +2493,10 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HLD/CDDs add to RTM
</commit_message>
<xml_diff>
--- a/management/RTM.xlsx
+++ b/management/RTM.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA_Embedded_project\Kenovo_ElectricBlender\management\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9336" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="9330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
     <sheet name="SRS" sheetId="4" r:id="rId4"/>
     <sheet name="Test Cases" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +28,7 @@
     <author>eze3</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment ref="A3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -148,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
+    <comment ref="F3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
   <si>
     <t>REQUIREMENTS TRACEABILITY MATRIX</t>
   </si>
@@ -261,7 +256,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -276,7 +271,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -291,7 +286,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -326,7 +321,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -341,7 +336,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -356,7 +351,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -393,7 +388,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -598,6 +593,18 @@
   <si>
     <t>speeds variation must be observed clearly by vision and sound</t>
   </si>
+  <si>
+    <t xml:space="preserve">HLD_02
+HLD_05
+HLD_07
+</t>
+  </si>
+  <si>
+    <t>HLD_01
+HLD_04
+HLD_06
+HLD_07</t>
+  </si>
 </sst>
 </file>
 
@@ -607,7 +614,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -644,7 +651,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -677,7 +684,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -691,7 +698,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -722,7 +729,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -897,6 +904,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -937,10 +948,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1025,7 +1032,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1060,7 +1067,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1237,7 +1244,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1251,64 +1258,64 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="30.75" customWidth="1"/>
+    <col min="2" max="2" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:1" s="20" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+    <row r="2" spans="1:1" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:1" s="22" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="20" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:1" s="22" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:1" s="22" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="22" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:1" s="24" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:1" s="22" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="20" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:1" s="22" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="20" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:1" s="22" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="20" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:1" s="22" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="20" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:1" s="22" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A8:XFD8"/>
@@ -1331,51 +1338,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.21875" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" style="18" customWidth="1"/>
-    <col min="3" max="3" width="35.44140625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7.25" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="18" customWidth="1"/>
+    <col min="3" max="3" width="35.5" style="19" customWidth="1"/>
+    <col min="4" max="4" width="26.375" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" customWidth="1"/>
+    <col min="7" max="7" width="20.375" customWidth="1"/>
+    <col min="8" max="8" width="18.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="32"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1402,17 +1409,19 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="95.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>92</v>
+      </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
         <v>78</v>
@@ -1421,14 +1430,14 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="137.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="20" t="s">
         <v>89</v>
       </c>
       <c r="D5" s="7"/>
@@ -1440,17 +1449,19 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="129" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="129" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>93</v>
+      </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
         <v>80</v>
@@ -1459,7 +1470,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1472,7 +1483,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -1485,7 +1496,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
@@ -1498,7 +1509,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -1511,7 +1522,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -1524,7 +1535,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
@@ -1537,7 +1548,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
@@ -1550,7 +1561,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -1563,7 +1574,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -1576,7 +1587,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
@@ -1589,7 +1600,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="16"/>
       <c r="C17" s="7"/>
@@ -1600,7 +1611,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="17"/>
       <c r="C18" s="7"/>
@@ -1611,7 +1622,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="17"/>
       <c r="C19" s="7"/>
@@ -1622,7 +1633,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="17"/>
       <c r="C20" s="7"/>
@@ -1633,7 +1644,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="17"/>
       <c r="C21" s="7"/>
@@ -1644,7 +1655,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="17"/>
       <c r="C22" s="7"/>
@@ -1655,7 +1666,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="17"/>
       <c r="C23" s="7"/>
@@ -1666,7 +1677,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="17"/>
       <c r="C24" s="7"/>
@@ -1677,7 +1688,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="17"/>
       <c r="C25" s="7"/>
@@ -1688,7 +1699,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="17"/>
       <c r="C26" s="7"/>
@@ -1699,7 +1710,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="17"/>
       <c r="C27" s="7"/>
@@ -1710,7 +1721,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="17"/>
       <c r="C28" s="7"/>
@@ -1721,7 +1732,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="17"/>
       <c r="C29" s="7"/>
@@ -1732,7 +1743,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="17"/>
       <c r="C30" s="7"/>
@@ -1743,7 +1754,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="17"/>
       <c r="C31" s="7"/>
@@ -1754,7 +1765,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="17"/>
       <c r="C32" s="7"/>
@@ -1765,7 +1776,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="17"/>
       <c r="C33" s="7"/>
@@ -1776,7 +1787,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" s="17"/>
       <c r="C34" s="7"/>
@@ -1787,7 +1798,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="17"/>
       <c r="C35" s="7"/>
@@ -1798,7 +1809,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" s="17"/>
       <c r="C36" s="7"/>
@@ -1809,7 +1820,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="17"/>
       <c r="C37" s="7"/>
@@ -1820,7 +1831,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
       <c r="B38" s="17"/>
       <c r="C38" s="6"/>
@@ -1831,7 +1842,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="17"/>
       <c r="C39" s="6"/>
@@ -1842,7 +1853,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
       <c r="B40" s="17"/>
       <c r="C40" s="6"/>
@@ -1853,7 +1864,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="17"/>
       <c r="C41" s="6"/>
@@ -1864,7 +1875,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="B42" s="17"/>
       <c r="C42" s="6"/>
@@ -1875,7 +1886,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="17"/>
       <c r="C43" s="6"/>
@@ -1886,7 +1897,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
       <c r="B44" s="17"/>
       <c r="C44" s="6"/>
@@ -1897,7 +1908,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="17"/>
       <c r="C45" s="6"/>
@@ -1908,7 +1919,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" s="17"/>
       <c r="C46" s="6"/>
@@ -1919,7 +1930,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="17"/>
       <c r="C47" s="6"/>
@@ -1930,7 +1941,7 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="17"/>
       <c r="C48" s="6"/>
@@ -1941,7 +1952,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="17"/>
       <c r="C49" s="6"/>
@@ -1952,7 +1963,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
       <c r="B50" s="17"/>
       <c r="C50" s="6"/>
@@ -1963,7 +1974,7 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
       <c r="B51" s="17"/>
       <c r="C51" s="6"/>
@@ -1974,7 +1985,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="6"/>
       <c r="B52" s="17"/>
       <c r="C52" s="6"/>
@@ -1985,7 +1996,7 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
       <c r="B53" s="17"/>
       <c r="C53" s="6"/>
@@ -1996,7 +2007,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
       <c r="B54" s="17"/>
       <c r="C54" s="6"/>
@@ -2007,7 +2018,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
       <c r="B55" s="17"/>
       <c r="C55" s="6"/>
@@ -2018,7 +2029,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="6"/>
       <c r="B56" s="17"/>
       <c r="C56" s="6"/>
@@ -2029,7 +2040,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
       <c r="B57" s="17"/>
       <c r="C57" s="6"/>
@@ -2040,7 +2051,7 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="6"/>
       <c r="B58" s="17"/>
       <c r="C58" s="6"/>
@@ -2051,7 +2062,7 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
       <c r="B59" s="17"/>
       <c r="C59" s="6"/>
@@ -2062,7 +2073,7 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="6"/>
       <c r="B60" s="17"/>
       <c r="C60" s="6"/>
@@ -2073,7 +2084,7 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
       <c r="B61" s="17"/>
       <c r="C61" s="6"/>
@@ -2084,7 +2095,7 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="6"/>
       <c r="B62" s="17"/>
       <c r="C62" s="6"/>
@@ -2095,7 +2106,7 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="6"/>
       <c r="B63" s="17"/>
       <c r="C63" s="6"/>
@@ -2106,7 +2117,7 @@
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="6"/>
       <c r="B64" s="17"/>
       <c r="C64" s="6"/>
@@ -2117,7 +2128,7 @@
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="6"/>
       <c r="B65" s="17"/>
       <c r="C65" s="6"/>
@@ -2128,7 +2139,7 @@
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="6"/>
       <c r="B66" s="17"/>
       <c r="C66" s="6"/>
@@ -2172,16 +2183,16 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="74.44140625" customWidth="1"/>
+    <col min="2" max="2" width="74.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -2189,7 +2200,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -2197,7 +2208,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -2214,16 +2225,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>44</v>
       </c>
@@ -2231,7 +2242,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>45</v>
       </c>
@@ -2239,7 +2250,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>46</v>
       </c>
@@ -2247,7 +2258,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>47</v>
       </c>
@@ -2255,7 +2266,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>48</v>
       </c>
@@ -2263,15 +2274,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="21" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>50</v>
       </c>
@@ -2279,7 +2290,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>51</v>
       </c>
@@ -2287,7 +2298,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>52</v>
       </c>
@@ -2295,7 +2306,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>53</v>
       </c>
@@ -2303,7 +2314,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>54</v>
       </c>
@@ -2311,7 +2322,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>55</v>
       </c>
@@ -2333,13 +2344,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="26.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="26.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>56</v>
       </c>
@@ -2347,7 +2358,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>58</v>
       </c>
@@ -2355,7 +2366,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>60</v>
       </c>
@@ -2363,7 +2374,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>62</v>
       </c>
@@ -2371,103 +2382,103 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="35" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="31" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="35" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="31" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="35" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
-      <c r="B22" s="32"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="32"/>
-      <c r="B24" s="32"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>72</v>
       </c>
@@ -2475,11 +2486,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="13"/>
     </row>
-    <row r="27" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>74</v>
       </c>
@@ -2487,11 +2498,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="13"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Update RTM with Test Cases by Basma Emad.
</commit_message>
<xml_diff>
--- a/management/RTM.xlsx
+++ b/management/RTM.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iTi Software Testing and Quality Assurance\CM\Project\management\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="9330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="9330" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
     <author>eze3</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -143,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -171,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="110">
   <si>
     <t>REQUIREMENTS TRACEABILITY MATRIX</t>
   </si>
@@ -256,7 +261,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -271,7 +276,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -286,7 +291,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -321,7 +326,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -336,7 +341,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -351,7 +356,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -388,7 +393,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -465,57 +470,27 @@
     <t>TC_1</t>
   </si>
   <si>
-    <t xml:space="preserve"> validate button pressing</t>
-  </si>
-  <si>
     <t>TC_2</t>
   </si>
   <si>
-    <t xml:space="preserve"> validate Speed 1</t>
-  </si>
-  <si>
     <t>TC_3</t>
   </si>
   <si>
-    <t xml:space="preserve"> validate Speed 2</t>
-  </si>
-  <si>
     <t>TC_4</t>
   </si>
   <si>
-    <t xml:space="preserve"> validate Speed 3</t>
-  </si>
-  <si>
     <t>TC_5</t>
   </si>
   <si>
-    <t>Validate Pressing on button frequently.</t>
-  </si>
-  <si>
-    <t>TC_6</t>
-  </si>
-  <si>
     <t>Validate Long Press on the button.</t>
   </si>
   <si>
     <t>TC_7</t>
   </si>
   <si>
-    <t>validate motor rotation</t>
-  </si>
-  <si>
     <t>TC_8</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify Protection circuit </t>
-  </si>
-  <si>
-    <t>TC _9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify the PWM Voltage </t>
-  </si>
-  <si>
     <t>TC_10</t>
   </si>
   <si>
@@ -526,27 +501,6 @@
   </si>
   <si>
     <t>Verify No Power Button.</t>
-  </si>
-  <si>
-    <t>- TC_10 - 
-- TC_7 - 
-- TC_8 -  
-- TC_9 -  
-- TC_6 - 
-- TC_1 -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- TC_8 - 
-- TC_8 - 
-- TC_8 - 
-- TC_8 - </t>
-  </si>
-  <si>
-    <t>- TC_11 - 
-- TC_6 - 
-- TC_1 - 
-- TC_1 - 
-- TC_5 -</t>
   </si>
   <si>
     <t>Motor operating voltage is between 5 to 9V</t>
@@ -605,16 +559,116 @@
 HLD_06
 HLD_07</t>
   </si>
+  <si>
+    <t>TC ID</t>
+  </si>
+  <si>
+    <t>TC _ 6</t>
+  </si>
+  <si>
+    <t>TC_9</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>TC _13</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t>TC_15</t>
+  </si>
+  <si>
+    <t>TC_16</t>
+  </si>
+  <si>
+    <t>TC_17</t>
+  </si>
+  <si>
+    <t>TC_18</t>
+  </si>
+  <si>
+    <t>TC Title</t>
+  </si>
+  <si>
+    <t>Validate button pressing</t>
+  </si>
+  <si>
+    <t>Validate button pressing behavior</t>
+  </si>
+  <si>
+    <t>Validate Speed 1</t>
+  </si>
+  <si>
+    <t>Validate Speed 2</t>
+  </si>
+  <si>
+    <t>Validate Speed 3</t>
+  </si>
+  <si>
+    <t>Validate motor power supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate  short button pressing </t>
+  </si>
+  <si>
+    <t>Validate Pressing on button frequently</t>
+  </si>
+  <si>
+    <t>Validate action after button pressed and released</t>
+  </si>
+  <si>
+    <t>Validate voltage less than 5 volt</t>
+  </si>
+  <si>
+    <t>Validate voltage more than 9 volt</t>
+  </si>
+  <si>
+    <t>Verify the PWM Voltage</t>
+  </si>
+  <si>
+    <t>Validate motor rotation</t>
+  </si>
+  <si>
+    <t>Verify Protection circuit</t>
+  </si>
+  <si>
+    <t>Validate blender active unless the user changes the speed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- TC_3 - 
+- TC_4 - 
+- TC_5 - 
+- TC_13 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- TC_6, TC_11,TC_12 - 
+- TC_15- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- TC_16 - 
+- TC_14 - 
+- TC_17 -
+- TC_1,TC_9 -
+- TC_2 ,TC_8-
+- TC_8 -
+- TC_18 -
+- TC_2 -
+- TC_10 -
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -651,7 +705,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -684,7 +738,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -698,18 +752,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -729,12 +778,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -771,8 +829,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3D85C6"/>
+        <bgColor rgb="FF3D85C6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -847,6 +911,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -881,33 +958,26 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -941,11 +1011,20 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1244,7 +1323,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1258,64 +1337,64 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.75" customWidth="1"/>
-    <col min="2" max="2" width="8.75" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:1" s="22" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+    <row r="2" spans="1:1" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:1" s="19" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="22" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:1" s="19" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="22" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:1" s="19" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="24" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+    <row r="6" spans="1:1" s="21" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="22" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:1" s="19" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="22" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:1" s="19" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="22" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:1" s="19" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="22" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:1" s="19" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="22" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:1" s="19" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A8:XFD8"/>
@@ -1338,51 +1417,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.25" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="18" customWidth="1"/>
-    <col min="3" max="3" width="35.5" style="19" customWidth="1"/>
-    <col min="4" max="4" width="26.375" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="20.375" customWidth="1"/>
-    <col min="8" max="8" width="18.75" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1409,72 +1488,72 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="95.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="95.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>88</v>
+      <c r="C4" s="17" t="s">
+        <v>75</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="137.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="137.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>89</v>
+      <c r="C5" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="129" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>90</v>
+      <c r="C6" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1483,11 +1562,11 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1496,11 +1575,11 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1509,11 +1588,11 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1522,11 +1601,11 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1535,11 +1614,11 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1548,11 +1627,11 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1561,11 +1640,11 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1574,11 +1653,11 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="15"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1587,11 +1666,11 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1600,9 +1679,9 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="16"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1611,9 +1690,9 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="17"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1622,9 +1701,9 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="17"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1633,9 +1712,9 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="17"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -1644,9 +1723,9 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="17"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -1655,9 +1734,9 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="17"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -1666,9 +1745,9 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="17"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1677,9 +1756,9 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="17"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -1688,9 +1767,9 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="17"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -1699,9 +1778,9 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
-      <c r="B26" s="17"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -1710,9 +1789,9 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
-      <c r="B27" s="17"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -1721,9 +1800,9 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
-      <c r="B28" s="17"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -1732,9 +1811,9 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
-      <c r="B29" s="17"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
@@ -1743,9 +1822,9 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
-      <c r="B30" s="17"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
@@ -1754,9 +1833,9 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="B31" s="17"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -1765,9 +1844,9 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
-      <c r="B32" s="17"/>
+      <c r="B32" s="14"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -1776,9 +1855,9 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
-      <c r="B33" s="17"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -1787,9 +1866,9 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="17"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -1798,9 +1877,9 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
-      <c r="B35" s="17"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -1809,9 +1888,9 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
-      <c r="B36" s="17"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -1820,9 +1899,9 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
-      <c r="B37" s="17"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -1831,9 +1910,9 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
-      <c r="B38" s="17"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -1842,9 +1921,9 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
-      <c r="B39" s="17"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -1853,9 +1932,9 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
-      <c r="B40" s="17"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -1864,9 +1943,9 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
-      <c r="B41" s="17"/>
+      <c r="B41" s="14"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -1875,9 +1954,9 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="17"/>
+      <c r="B42" s="14"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -1886,9 +1965,9 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="17"/>
+      <c r="B43" s="14"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -1897,9 +1976,9 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
-      <c r="B44" s="17"/>
+      <c r="B44" s="14"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -1908,9 +1987,9 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
-      <c r="B45" s="17"/>
+      <c r="B45" s="14"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -1919,9 +1998,9 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
-      <c r="B46" s="17"/>
+      <c r="B46" s="14"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -1930,9 +2009,9 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
-      <c r="B47" s="17"/>
+      <c r="B47" s="14"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
@@ -1941,9 +2020,9 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
-      <c r="B48" s="17"/>
+      <c r="B48" s="14"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -1952,9 +2031,9 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
-      <c r="B49" s="17"/>
+      <c r="B49" s="14"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -1963,9 +2042,9 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
-      <c r="B50" s="17"/>
+      <c r="B50" s="14"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
@@ -1974,9 +2053,9 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
-      <c r="B51" s="17"/>
+      <c r="B51" s="14"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -1985,9 +2064,9 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
-      <c r="B52" s="17"/>
+      <c r="B52" s="14"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -1996,9 +2075,9 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
-      <c r="B53" s="17"/>
+      <c r="B53" s="14"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -2007,9 +2086,9 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
-      <c r="B54" s="17"/>
+      <c r="B54" s="14"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -2018,9 +2097,9 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
-      <c r="B55" s="17"/>
+      <c r="B55" s="14"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
@@ -2029,9 +2108,9 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
-      <c r="B56" s="17"/>
+      <c r="B56" s="14"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -2040,9 +2119,9 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
-      <c r="B57" s="17"/>
+      <c r="B57" s="14"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
@@ -2051,9 +2130,9 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
-      <c r="B58" s="17"/>
+      <c r="B58" s="14"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
@@ -2062,9 +2141,9 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
-      <c r="B59" s="17"/>
+      <c r="B59" s="14"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
@@ -2073,9 +2152,9 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
-      <c r="B60" s="17"/>
+      <c r="B60" s="14"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
@@ -2084,9 +2163,9 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
-      <c r="B61" s="17"/>
+      <c r="B61" s="14"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
@@ -2095,9 +2174,9 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
-      <c r="B62" s="17"/>
+      <c r="B62" s="14"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
@@ -2106,9 +2185,9 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
-      <c r="B63" s="17"/>
+      <c r="B63" s="14"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
@@ -2117,9 +2196,9 @@
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
-      <c r="B64" s="17"/>
+      <c r="B64" s="14"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
@@ -2128,9 +2207,9 @@
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
-      <c r="B65" s="17"/>
+      <c r="B65" s="14"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
@@ -2139,9 +2218,9 @@
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
-      <c r="B66" s="17"/>
+      <c r="B66" s="14"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
@@ -2186,13 +2265,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="74.5" customWidth="1"/>
+    <col min="2" max="2" width="74.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -2200,7 +2279,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -2208,7 +2287,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -2229,105 +2308,105 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.875" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="B4" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="B5" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="B6" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="B7" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="B8" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="B9" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="B10" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>87</v>
+      <c r="B12" s="16" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2338,189 +2417,219 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="26.75" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B3" s="31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="B4" s="31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B5" s="31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="B6" s="31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B7" s="31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+    <row r="13" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B13" s="32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="31" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="35" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="35" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="13"/>
-    </row>
-    <row r="27" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-      <c r="B28" s="13"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>77</v>
-      </c>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
+    </row>
+    <row r="30" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="B10:B14"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>